<commit_message>
Major update to export_hpop_country_summary_xls to output flexible data sheets
</commit_message>
<xml_diff>
--- a/data-raw/CountrySummary_Template.xlsx
+++ b/data-raw/CountrySummary_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F446662-6353-46A1-BB9A-703CC24ECDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D19D398-582C-40B0-BDF1-E4C62339FA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="601" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="17640" tabRatio="601" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
   <sheets>
     <sheet name="HPOPdata" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="HPOPIndicator List" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HPOPdata!$A$1:$R$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">HPOPdata!$A$1:$Q$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
   <si>
     <t>Magnitude +</t>
   </si>
@@ -81,27 +81,6 @@
     <t>Adult Obesity</t>
   </si>
   <si>
-    <t>Contribution to the Billion</t>
-  </si>
-  <si>
-    <t>Raw Value</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Indicators</t>
-  </si>
-  <si>
-    <t>Number of Values (Since 2000)</t>
-  </si>
-  <si>
     <t>Adolescent/ Child Obesity</t>
   </si>
   <si>
@@ -183,51 +162,18 @@
     <t>Year Lastest</t>
   </si>
   <si>
-    <t>Country name</t>
-  </si>
-  <si>
     <t>Transformed Indicator</t>
   </si>
   <si>
-    <t>Change in Transformed Values over 2018-2023)- %</t>
-  </si>
-  <si>
-    <t>UN Population 2023- Thousands</t>
-  </si>
-  <si>
     <t>Time Series</t>
   </si>
   <si>
-    <t>Latest Reported/Estimated Data Available</t>
-  </si>
-  <si>
-    <t>Number of Values (Since 2012)</t>
-  </si>
-  <si>
     <t>* For a number of countries Safely Managed Water and Safely Managed Sanitation were measured for the urban or rural population (not the total population).</t>
   </si>
   <si>
     <t>Note: The value for the latest year available prior to 2018 was transformed depending on the indicators (see HPOP data spreadsheet).</t>
   </si>
   <si>
-    <t>Contribution 2023 - Thousands</t>
-  </si>
-  <si>
-    <t>Contribution 2023 - % Total Population</t>
-  </si>
-  <si>
-    <t>Country contribution to GPW13 BILLION_NAME billion target</t>
-  </si>
-  <si>
-    <t>2018 Baselines, and 2023 and Projections</t>
-  </si>
-  <si>
-    <t>Indicator transformed</t>
-  </si>
-  <si>
-    <t>Unit transformed</t>
-  </si>
-  <si>
     <t>Indicator code</t>
   </si>
   <si>
@@ -355,9 +301,6 @@
   </si>
   <si>
     <t>Time Series (Transformed Values)</t>
-  </si>
-  <si>
-    <t>Transformed Value</t>
   </si>
 </sst>
 </file>
@@ -367,7 +310,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,31 +335,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="6"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -425,14 +344,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -463,37 +374,6 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -536,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -572,15 +452,6 @@
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -636,45 +507,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -692,19 +524,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
@@ -719,17 +541,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -738,19 +556,19 @@
       <alignment horizontal="right" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -760,50 +578,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -815,65 +603,17 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2013,7 +1753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{961EA231-1DF3-4463-9644-B6FAC907A867}" type="CELLRANGE">
+                    <a:fld id="{6071C4AC-2F6D-4B20-A20D-30CCF9C33A66}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2784,1058 +2524,111 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AH73"/>
+  <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.85546875" style="41" customWidth="1"/>
-    <col min="4" max="5" width="6.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="0.85546875" style="41" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="0.85546875" style="41" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="6.5703125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" style="3" customWidth="1"/>
-    <col min="23" max="23" width="47.85546875" style="1" customWidth="1"/>
-    <col min="24" max="25" width="10.140625" style="1" customWidth="1"/>
-    <col min="26" max="34" width="9.140625" style="31"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="0.85546875" customWidth="1"/>
+    <col min="4" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="11" width="24.7109375" customWidth="1"/>
+    <col min="12" max="12" width="0.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="0.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="6.5703125" customWidth="1"/>
+    <col min="21" max="21" width="11.85546875" customWidth="1"/>
+    <col min="22" max="22" width="47.85546875" customWidth="1"/>
+    <col min="23" max="24" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="31" customFormat="1">
-      <c r="A1" s="32"/>
-      <c r="C1" s="38"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="R1" s="38"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
-    </row>
-    <row r="2" spans="1:34" s="31" customFormat="1" ht="30" customHeight="1">
-      <c r="A2" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="R2" s="38"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="33"/>
-    </row>
-    <row r="3" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="32"/>
-      <c r="C3" s="38"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="R3" s="38"/>
-      <c r="U3" s="32"/>
-      <c r="V3" s="33"/>
-    </row>
-    <row r="4" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="R4" s="38"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="33"/>
-    </row>
-    <row r="5" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="33"/>
-      <c r="Y5" s="38"/>
-    </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1">
-      <c r="A6" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="T6" s="68"/>
-      <c r="U6" s="68"/>
-      <c r="V6" s="68"/>
-      <c r="W6" s="68"/>
-      <c r="X6" s="68"/>
-      <c r="Y6" s="71"/>
-    </row>
-    <row r="7" spans="1:34" ht="30" customHeight="1">
-      <c r="A7" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="64"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="64" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="61"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" s="62" t="s">
-        <v>50</v>
-      </c>
-      <c r="P7" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q7" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="R7" s="40"/>
-      <c r="S7" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="T7" s="72" t="s">
-        <v>105</v>
-      </c>
-      <c r="U7" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="V7" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="W7" s="72" t="s">
-        <v>17</v>
-      </c>
-      <c r="X7" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y7" s="72" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" ht="15" customHeight="1">
-      <c r="A8" s="70"/>
-      <c r="B8" s="59"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="50">
-        <v>2018</v>
-      </c>
-      <c r="E8" s="50">
-        <v>2023</v>
-      </c>
-      <c r="F8" s="49"/>
-      <c r="G8" s="50">
-        <v>2018</v>
-      </c>
-      <c r="H8" s="50">
-        <v>2023</v>
-      </c>
-      <c r="I8" s="50">
-        <v>2018</v>
-      </c>
-      <c r="J8" s="50">
-        <v>2023</v>
-      </c>
-      <c r="K8" s="50">
-        <v>2018</v>
-      </c>
-      <c r="L8" s="50">
-        <v>2023</v>
-      </c>
-      <c r="M8" s="40"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="59"/>
-      <c r="R8" s="40"/>
-      <c r="S8" s="59"/>
-      <c r="T8" s="59"/>
-      <c r="U8" s="59"/>
-      <c r="V8" s="59"/>
-      <c r="W8" s="59"/>
-      <c r="X8" s="59"/>
-      <c r="Y8" s="59"/>
-    </row>
-    <row r="9" spans="1:34" s="14" customFormat="1" ht="30" customHeight="1">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
-      <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9" s="31"/>
-      <c r="AA9" s="31"/>
-      <c r="AB9" s="31"/>
-      <c r="AC9" s="31"/>
-      <c r="AD9" s="31"/>
-      <c r="AE9" s="31"/>
-      <c r="AF9" s="31"/>
-      <c r="AG9" s="31"/>
-      <c r="AH9" s="31"/>
-    </row>
-    <row r="10" spans="1:34" ht="30" customHeight="1">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-    </row>
-    <row r="11" spans="1:34" ht="30" customHeight="1">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
-      <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-    </row>
-    <row r="12" spans="1:34" ht="30" customHeight="1">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-      <c r="R12"/>
-      <c r="S12"/>
-      <c r="T12"/>
-      <c r="U12"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-    </row>
-    <row r="13" spans="1:34" ht="30" customHeight="1">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="S13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-    </row>
-    <row r="14" spans="1:34" ht="30" customHeight="1">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-      <c r="R14"/>
-      <c r="S14"/>
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
-      <c r="Y14"/>
-    </row>
-    <row r="15" spans="1:34" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
-      <c r="S15"/>
-      <c r="T15"/>
-      <c r="U15"/>
-      <c r="V15"/>
-      <c r="W15"/>
-      <c r="X15"/>
-      <c r="Y15"/>
-      <c r="Z15" s="31"/>
-      <c r="AA15" s="31"/>
-      <c r="AB15" s="31"/>
-      <c r="AC15" s="31"/>
-      <c r="AD15" s="31"/>
-      <c r="AE15" s="31"/>
-      <c r="AF15" s="31"/>
-      <c r="AG15" s="31"/>
-      <c r="AH15" s="31"/>
-    </row>
-    <row r="16" spans="1:34" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-      <c r="Y16"/>
-      <c r="Z16" s="31"/>
-      <c r="AA16" s="31"/>
-      <c r="AB16" s="31"/>
-      <c r="AC16" s="31"/>
-      <c r="AD16" s="31"/>
-      <c r="AE16" s="31"/>
-      <c r="AF16" s="31"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="31"/>
-    </row>
-    <row r="17" spans="1:34" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-      <c r="N17"/>
-      <c r="O17"/>
-      <c r="P17"/>
-      <c r="Q17"/>
-      <c r="R17"/>
-      <c r="S17"/>
-      <c r="T17"/>
-      <c r="U17"/>
-      <c r="V17"/>
-      <c r="W17"/>
-      <c r="X17"/>
-      <c r="Y17"/>
-      <c r="Z17" s="31"/>
-      <c r="AA17" s="31"/>
-      <c r="AB17" s="31"/>
-      <c r="AC17" s="31"/>
-      <c r="AD17" s="31"/>
-      <c r="AE17" s="31"/>
-      <c r="AF17" s="31"/>
-      <c r="AG17" s="31"/>
-      <c r="AH17" s="31"/>
-    </row>
-    <row r="18" spans="1:34" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="R18"/>
-      <c r="S18"/>
-      <c r="T18"/>
-      <c r="U18"/>
-      <c r="V18"/>
-      <c r="W18"/>
-      <c r="X18"/>
-      <c r="Y18"/>
-      <c r="Z18" s="31"/>
-      <c r="AA18" s="31"/>
-      <c r="AB18" s="31"/>
-      <c r="AC18" s="31"/>
-      <c r="AD18" s="31"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
-    </row>
-    <row r="19" spans="1:34" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
-      <c r="S19"/>
-      <c r="T19"/>
-      <c r="U19"/>
-      <c r="V19"/>
-      <c r="W19"/>
-      <c r="X19"/>
-      <c r="Y19"/>
-      <c r="Z19" s="31"/>
-      <c r="AA19" s="31"/>
-      <c r="AB19" s="31"/>
-      <c r="AC19" s="31"/>
-      <c r="AD19" s="31"/>
-      <c r="AE19" s="31"/>
-      <c r="AF19" s="31"/>
-      <c r="AG19" s="31"/>
-      <c r="AH19" s="31"/>
-    </row>
-    <row r="20" spans="1:34" ht="30" customHeight="1">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="P20"/>
-      <c r="Q20"/>
-      <c r="R20"/>
-      <c r="S20"/>
-      <c r="T20"/>
-      <c r="U20"/>
-      <c r="V20"/>
-      <c r="W20"/>
-      <c r="X20"/>
-      <c r="Y20"/>
-    </row>
-    <row r="21" spans="1:34" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-      <c r="N21"/>
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-      <c r="R21"/>
-      <c r="S21"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
-      <c r="W21"/>
-      <c r="X21"/>
-      <c r="Y21"/>
-      <c r="Z21" s="31"/>
-      <c r="AA21" s="31"/>
-      <c r="AB21" s="31"/>
-      <c r="AC21" s="31"/>
-      <c r="AD21" s="31"/>
-      <c r="AE21" s="31"/>
-      <c r="AF21" s="31"/>
-      <c r="AG21" s="31"/>
-      <c r="AH21" s="31"/>
-    </row>
-    <row r="22" spans="1:34" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22"/>
-      <c r="T22"/>
-      <c r="U22"/>
-      <c r="V22"/>
-      <c r="W22"/>
-      <c r="X22"/>
-      <c r="Y22"/>
-      <c r="Z22" s="31"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="31"/>
-      <c r="AC22" s="31"/>
-      <c r="AD22" s="31"/>
-      <c r="AE22" s="31"/>
-      <c r="AF22" s="31"/>
-      <c r="AG22" s="31"/>
-      <c r="AH22" s="31"/>
-    </row>
-    <row r="23" spans="1:34" s="5" customFormat="1" ht="30" customHeight="1">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-      <c r="N23"/>
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
-      <c r="S23"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
-      <c r="W23"/>
-      <c r="X23"/>
-      <c r="Y23"/>
-      <c r="Z23" s="31"/>
-      <c r="AA23" s="31"/>
-      <c r="AB23" s="31"/>
-      <c r="AC23" s="31"/>
-      <c r="AD23" s="31"/>
-      <c r="AE23" s="31"/>
-      <c r="AF23" s="31"/>
-      <c r="AG23" s="31"/>
-      <c r="AH23" s="31"/>
-    </row>
-    <row r="24" spans="1:34" s="6" customFormat="1" ht="30" customHeight="1">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-      <c r="N24"/>
-      <c r="O24"/>
-      <c r="P24"/>
-      <c r="Q24"/>
-      <c r="R24"/>
-      <c r="S24"/>
-      <c r="T24"/>
-      <c r="U24"/>
-      <c r="V24"/>
-      <c r="W24"/>
-      <c r="X24"/>
-      <c r="Y24"/>
-      <c r="Z24" s="31"/>
-      <c r="AA24" s="31"/>
-      <c r="AB24" s="31"/>
-      <c r="AC24" s="31"/>
-      <c r="AD24" s="31"/>
-      <c r="AE24" s="31"/>
-      <c r="AF24" s="31"/>
-      <c r="AG24" s="31"/>
-      <c r="AH24" s="31"/>
-    </row>
-    <row r="25" spans="1:34" s="6" customFormat="1" ht="30" customHeight="1">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25"/>
-      <c r="P25"/>
-      <c r="Q25"/>
-      <c r="R25"/>
-      <c r="S25"/>
-      <c r="T25"/>
-      <c r="U25"/>
-      <c r="V25"/>
-      <c r="W25"/>
-      <c r="X25"/>
-      <c r="Y25"/>
-      <c r="Z25" s="31"/>
-      <c r="AA25" s="31"/>
-      <c r="AB25" s="31"/>
-      <c r="AC25" s="31"/>
-      <c r="AD25" s="31"/>
-      <c r="AE25" s="31"/>
-      <c r="AF25" s="31"/>
-      <c r="AG25" s="31"/>
-      <c r="AH25" s="31"/>
-    </row>
-    <row r="26" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N26" s="26"/>
-      <c r="P26" s="48"/>
-      <c r="Q26" s="48"/>
-    </row>
-    <row r="27" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N27" s="26"/>
-      <c r="P27" s="48"/>
-      <c r="Q27" s="48"/>
-    </row>
-    <row r="28" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N28" s="26"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="48"/>
-    </row>
-    <row r="29" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N29" s="26"/>
-      <c r="P29" s="48"/>
-      <c r="Q29" s="48"/>
-    </row>
-    <row r="30" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N30" s="26"/>
-      <c r="P30" s="48"/>
-      <c r="Q30" s="48"/>
-    </row>
-    <row r="31" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N31" s="26"/>
-      <c r="P31" s="48"/>
-      <c r="Q31" s="48"/>
-    </row>
-    <row r="32" spans="1:34" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N32" s="26"/>
-      <c r="P32" s="48"/>
-      <c r="Q32" s="48"/>
-    </row>
-    <row r="33" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N33" s="26"/>
-      <c r="P33" s="48"/>
-      <c r="Q33" s="48"/>
-    </row>
-    <row r="34" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N34" s="26"/>
-      <c r="P34" s="48"/>
-      <c r="Q34" s="48"/>
-    </row>
-    <row r="35" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N35" s="26"/>
-      <c r="P35" s="48"/>
-      <c r="Q35" s="48"/>
-    </row>
-    <row r="36" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N36" s="26"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-    </row>
-    <row r="37" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N37" s="26"/>
-      <c r="P37" s="48"/>
-      <c r="Q37" s="48"/>
-    </row>
-    <row r="38" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N38" s="26"/>
-      <c r="P38" s="48"/>
-      <c r="Q38" s="48"/>
-    </row>
-    <row r="39" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N39" s="26"/>
-      <c r="P39" s="48"/>
-      <c r="Q39" s="48"/>
-    </row>
-    <row r="40" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N40" s="26"/>
-      <c r="P40" s="48"/>
-      <c r="Q40" s="48"/>
-    </row>
-    <row r="41" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N41" s="26"/>
-      <c r="P41" s="48"/>
-      <c r="Q41" s="48"/>
-    </row>
-    <row r="42" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N42" s="26"/>
-      <c r="P42" s="48"/>
-      <c r="Q42" s="48"/>
-    </row>
-    <row r="43" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N43" s="26"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-    </row>
-    <row r="44" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N44" s="26"/>
-      <c r="P44" s="48"/>
-      <c r="Q44" s="48"/>
-    </row>
-    <row r="45" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N45" s="26"/>
-      <c r="P45" s="48"/>
-      <c r="Q45" s="48"/>
-    </row>
-    <row r="46" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N46" s="26"/>
-      <c r="P46" s="48"/>
-      <c r="Q46" s="48"/>
-    </row>
-    <row r="47" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N47" s="26"/>
-      <c r="P47" s="48"/>
-      <c r="Q47" s="48"/>
-    </row>
-    <row r="48" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N48" s="26"/>
-      <c r="P48" s="48"/>
-      <c r="Q48" s="48"/>
-    </row>
-    <row r="49" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N49" s="26"/>
-      <c r="P49" s="48"/>
-      <c r="Q49" s="48"/>
-    </row>
-    <row r="50" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N50" s="26"/>
-      <c r="P50" s="48"/>
-      <c r="Q50" s="48"/>
-    </row>
-    <row r="51" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N51" s="26"/>
-      <c r="P51" s="48"/>
-      <c r="Q51" s="48"/>
-    </row>
-    <row r="52" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N52" s="26"/>
-      <c r="P52" s="48"/>
-      <c r="Q52" s="48"/>
-    </row>
-    <row r="53" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N53" s="26"/>
-      <c r="P53" s="48"/>
-      <c r="Q53" s="48"/>
-    </row>
-    <row r="54" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N54" s="26"/>
-      <c r="P54" s="48"/>
-      <c r="Q54" s="48"/>
-    </row>
-    <row r="55" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N55" s="26"/>
-      <c r="P55" s="48"/>
-      <c r="Q55" s="48"/>
-    </row>
-    <row r="56" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N56" s="26"/>
-      <c r="P56" s="48"/>
-      <c r="Q56" s="48"/>
-    </row>
-    <row r="57" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N57" s="26"/>
-      <c r="P57" s="48"/>
-      <c r="Q57" s="48"/>
-    </row>
-    <row r="58" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N58" s="26"/>
-      <c r="P58" s="48"/>
-      <c r="Q58" s="48"/>
-    </row>
-    <row r="59" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N59" s="26"/>
-      <c r="P59" s="48"/>
-      <c r="Q59" s="48"/>
-    </row>
-    <row r="60" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N60" s="26"/>
-      <c r="P60" s="48"/>
-      <c r="Q60" s="48"/>
-    </row>
-    <row r="61" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N61" s="26"/>
-      <c r="P61" s="48"/>
-      <c r="Q61" s="48"/>
-    </row>
-    <row r="62" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N62" s="26"/>
-      <c r="P62" s="48"/>
-      <c r="Q62" s="48"/>
-    </row>
-    <row r="63" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N63" s="26"/>
-      <c r="P63" s="48"/>
-      <c r="Q63" s="48"/>
-    </row>
-    <row r="64" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N64" s="26"/>
-      <c r="P64" s="48"/>
-      <c r="Q64" s="48"/>
-    </row>
-    <row r="65" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N65" s="26"/>
-      <c r="P65" s="48"/>
-      <c r="Q65" s="48"/>
-    </row>
-    <row r="66" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N66" s="26"/>
-      <c r="P66" s="48"/>
-      <c r="Q66" s="48"/>
-    </row>
-    <row r="67" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N67" s="26"/>
-      <c r="P67" s="48"/>
-      <c r="Q67" s="48"/>
-    </row>
-    <row r="68" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N68" s="26"/>
-      <c r="P68" s="48"/>
-      <c r="Q68" s="48"/>
-    </row>
-    <row r="69" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N69" s="26"/>
-      <c r="P69" s="48"/>
-      <c r="Q69" s="48"/>
-    </row>
-    <row r="70" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N70" s="26"/>
-      <c r="P70" s="48"/>
-      <c r="Q70" s="48"/>
-    </row>
-    <row r="71" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N71" s="26"/>
-      <c r="P71" s="48"/>
-      <c r="Q71" s="48"/>
-    </row>
-    <row r="72" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N72" s="26"/>
-      <c r="P72" s="48"/>
-      <c r="Q72" s="48"/>
-    </row>
-    <row r="73" spans="14:17" s="31" customFormat="1" ht="15" customHeight="1">
-      <c r="N73" s="26"/>
-      <c r="P73" s="48"/>
-      <c r="Q73" s="48"/>
-    </row>
+    <row r="1" customFormat="1"/>
+    <row r="2" customFormat="1" ht="30" customHeight="1"/>
+    <row r="3" customFormat="1" ht="15" customHeight="1"/>
+    <row r="4" customFormat="1" ht="15" customHeight="1"/>
+    <row r="5" customFormat="1" ht="15" customHeight="1"/>
+    <row r="6" customFormat="1" ht="15" customHeight="1"/>
+    <row r="7" customFormat="1" ht="30" customHeight="1"/>
+    <row r="8" customFormat="1" ht="15" customHeight="1"/>
+    <row r="9" customFormat="1" ht="30" customHeight="1"/>
+    <row r="10" customFormat="1" ht="30" customHeight="1"/>
+    <row r="11" customFormat="1" ht="30" customHeight="1"/>
+    <row r="12" customFormat="1" ht="30" customHeight="1"/>
+    <row r="13" customFormat="1" ht="30" customHeight="1"/>
+    <row r="14" customFormat="1" ht="30" customHeight="1"/>
+    <row r="15" customFormat="1" ht="30" customHeight="1"/>
+    <row r="16" customFormat="1" ht="30" customHeight="1"/>
+    <row r="17" customFormat="1" ht="30" customHeight="1"/>
+    <row r="18" customFormat="1" ht="30" customHeight="1"/>
+    <row r="19" customFormat="1" ht="30" customHeight="1"/>
+    <row r="20" customFormat="1" ht="30" customHeight="1"/>
+    <row r="21" customFormat="1" ht="30" customHeight="1"/>
+    <row r="22" customFormat="1" ht="30" customHeight="1"/>
+    <row r="23" customFormat="1" ht="30" customHeight="1"/>
+    <row r="24" customFormat="1" ht="30" customHeight="1"/>
+    <row r="25" customFormat="1" ht="30" customHeight="1"/>
+    <row r="26" customFormat="1" ht="15" customHeight="1"/>
+    <row r="27" customFormat="1" ht="15" customHeight="1"/>
+    <row r="28" customFormat="1" ht="15" customHeight="1"/>
+    <row r="29" customFormat="1" ht="15" customHeight="1"/>
+    <row r="30" customFormat="1" ht="15" customHeight="1"/>
+    <row r="31" customFormat="1" ht="15" customHeight="1"/>
+    <row r="32" customFormat="1" ht="15" customHeight="1"/>
+    <row r="33" customFormat="1" ht="15" customHeight="1"/>
+    <row r="34" customFormat="1" ht="15" customHeight="1"/>
+    <row r="35" customFormat="1" ht="15" customHeight="1"/>
+    <row r="36" customFormat="1" ht="15" customHeight="1"/>
+    <row r="37" customFormat="1" ht="15" customHeight="1"/>
+    <row r="38" customFormat="1" ht="15" customHeight="1"/>
+    <row r="39" customFormat="1" ht="15" customHeight="1"/>
+    <row r="40" customFormat="1" ht="15" customHeight="1"/>
+    <row r="41" customFormat="1" ht="15" customHeight="1"/>
+    <row r="42" customFormat="1" ht="15" customHeight="1"/>
+    <row r="43" customFormat="1" ht="15" customHeight="1"/>
+    <row r="44" customFormat="1" ht="15" customHeight="1"/>
+    <row r="45" customFormat="1" ht="15" customHeight="1"/>
+    <row r="46" customFormat="1" ht="15" customHeight="1"/>
+    <row r="47" customFormat="1" ht="15" customHeight="1"/>
+    <row r="48" customFormat="1" ht="15" customHeight="1"/>
+    <row r="49" customFormat="1" ht="15" customHeight="1"/>
+    <row r="50" customFormat="1" ht="15" customHeight="1"/>
+    <row r="51" customFormat="1" ht="15" customHeight="1"/>
+    <row r="52" customFormat="1" ht="15" customHeight="1"/>
+    <row r="53" customFormat="1" ht="15" customHeight="1"/>
+    <row r="54" customFormat="1" ht="15" customHeight="1"/>
+    <row r="55" customFormat="1" ht="15" customHeight="1"/>
+    <row r="56" customFormat="1" ht="15" customHeight="1"/>
+    <row r="57" customFormat="1" ht="15" customHeight="1"/>
+    <row r="58" customFormat="1" ht="15" customHeight="1"/>
+    <row r="59" customFormat="1" ht="15" customHeight="1"/>
+    <row r="60" customFormat="1" ht="15" customHeight="1"/>
+    <row r="61" customFormat="1" ht="15" customHeight="1"/>
+    <row r="62" customFormat="1" ht="15" customHeight="1"/>
+    <row r="63" customFormat="1" ht="15" customHeight="1"/>
+    <row r="64" customFormat="1" ht="15" customHeight="1"/>
+    <row r="65" customFormat="1" ht="15" customHeight="1"/>
+    <row r="66" customFormat="1" ht="15" customHeight="1"/>
+    <row r="67" customFormat="1" ht="15" customHeight="1"/>
+    <row r="68" customFormat="1" ht="15" customHeight="1"/>
+    <row r="69" customFormat="1" ht="15" customHeight="1"/>
+    <row r="70" customFormat="1" ht="15" customHeight="1"/>
+    <row r="71" customFormat="1" ht="15" customHeight="1"/>
+    <row r="72" customFormat="1" ht="15" customHeight="1"/>
+    <row r="73" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="S6:Y6"/>
-    <mergeCell ref="S7:S8"/>
-    <mergeCell ref="T7:T8"/>
-    <mergeCell ref="U7:U8"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="W7:W8"/>
-    <mergeCell ref="X7:X8"/>
-    <mergeCell ref="Y7:Y8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D6:L6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:E7"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3853,83 +2646,83 @@
   <sheetData>
     <row r="21" spans="2:20" ht="33.75" customHeight="1"/>
     <row r="22" spans="2:20" ht="162" customHeight="1">
-      <c r="B22" s="13"/>
-      <c r="C22" s="12" t="str">
+      <c r="B22" s="7"/>
+      <c r="C22" s="6" t="str">
         <f>HPOPInter!A3</f>
         <v>Children not stunted</v>
       </c>
-      <c r="D22" s="12" t="str">
+      <c r="D22" s="6" t="str">
         <f>HPOPInter!A4</f>
         <v>Children not wasted</v>
       </c>
-      <c r="E22" s="12" t="str">
+      <c r="E22" s="6" t="str">
         <f>HPOPInter!A5</f>
         <v>Children not overweight</v>
       </c>
-      <c r="F22" s="12" t="str">
+      <c r="F22" s="6" t="str">
         <f>HPOPInter!A6</f>
         <v>Developmentally on track under 5</v>
       </c>
-      <c r="G22" s="12" t="str">
+      <c r="G22" s="6" t="str">
         <f>HPOPInter!A7</f>
         <v>Children not obese</v>
       </c>
-      <c r="H22" s="12" t="str">
+      <c r="H22" s="6" t="str">
         <f>HPOPInter!A8</f>
         <v>Reduced partner violence</v>
       </c>
-      <c r="I22" s="12" t="str">
+      <c r="I22" s="6" t="str">
         <f>HPOPInter!A9</f>
         <v>Reduced child violence</v>
       </c>
-      <c r="J22" s="12" t="str">
+      <c r="J22" s="6" t="str">
         <f>HPOPInter!A10</f>
         <v>Reduced suicide attempts</v>
       </c>
-      <c r="K22" s="12" t="str">
+      <c r="K22" s="6" t="str">
         <f>HPOPInter!A11</f>
         <v>Road safety</v>
       </c>
-      <c r="L22" s="12" t="str">
+      <c r="L22" s="6" t="str">
         <f>HPOPInter!A12</f>
         <v>Safely managed water</v>
       </c>
-      <c r="M22" s="12" t="str">
+      <c r="M22" s="6" t="str">
         <f>HPOPInter!A13</f>
         <v>Safely managed sanitation</v>
       </c>
-      <c r="N22" s="12" t="str">
+      <c r="N22" s="6" t="str">
         <f>HPOPInter!A14</f>
         <v>Clean household fuels</v>
       </c>
-      <c r="O22" s="12" t="str">
+      <c r="O22" s="6" t="str">
         <f>HPOPInter!A15</f>
         <v>Reduced alcohol use</v>
       </c>
-      <c r="P22" s="12" t="str">
+      <c r="P22" s="6" t="str">
         <f>HPOPInter!A16</f>
         <v>Ambient air quality</v>
       </c>
-      <c r="Q22" s="12" t="str">
+      <c r="Q22" s="6" t="str">
         <f>HPOPInter!A17</f>
         <v>Tobacco non-use</v>
       </c>
-      <c r="R22" s="12" t="str">
+      <c r="R22" s="6" t="str">
         <f>HPOPInter!A18</f>
         <v>Adults not obese</v>
       </c>
-      <c r="S22" s="12" t="str">
+      <c r="S22" s="6" t="str">
         <f>HPOPInter!A19</f>
         <v>Healthy fats</v>
       </c>
-      <c r="T22" s="13"/>
+      <c r="T22" s="7"/>
     </row>
     <row r="23" spans="2:20">
       <c r="B23" s="1"/>
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3952,222 +2745,222 @@
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="26" customFormat="1">
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="30"/>
-    </row>
-    <row r="2" spans="1:39" s="26" customFormat="1" ht="21">
-      <c r="B2" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="29"/>
-    </row>
-    <row r="3" spans="1:39" s="26" customFormat="1">
-      <c r="B3" s="43"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
+    <row r="1" spans="1:39" s="18" customFormat="1">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="21"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="22"/>
+    </row>
+    <row r="2" spans="1:39" s="18" customFormat="1" ht="21">
+      <c r="B2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+    </row>
+    <row r="3" spans="1:39" s="18" customFormat="1">
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="26"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="26"/>
     </row>
     <row r="4" spans="1:39">
-      <c r="A4" s="26"/>
-      <c r="B4" s="73" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="60"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="60"/>
-      <c r="V4" s="60"/>
-      <c r="W4" s="60"/>
-      <c r="X4" s="60"/>
-      <c r="Y4" s="60"/>
-      <c r="Z4" s="60"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="26"/>
-      <c r="AJ4" s="26"/>
-      <c r="AK4" s="26"/>
-      <c r="AL4" s="26"/>
-      <c r="AM4" s="26"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="18"/>
+      <c r="AK4" s="18"/>
+      <c r="AL4" s="18"/>
+      <c r="AM4" s="18"/>
     </row>
     <row r="5" spans="1:39">
-      <c r="A5" s="26"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="46">
+      <c r="A5" s="18"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="27">
         <v>2000</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="28">
         <v>2001</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="28">
         <v>2002</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="28">
         <v>2003</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="28">
         <v>2004</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="28">
         <v>2005</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="28">
         <v>2006</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="28">
         <v>2007</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="28">
         <v>2008</v>
       </c>
-      <c r="L5" s="47">
+      <c r="L5" s="28">
         <v>2009</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="28">
         <v>2010</v>
       </c>
-      <c r="N5" s="47">
+      <c r="N5" s="28">
         <v>2011</v>
       </c>
-      <c r="O5" s="47">
+      <c r="O5" s="28">
         <v>2012</v>
       </c>
-      <c r="P5" s="47">
+      <c r="P5" s="28">
         <v>2013</v>
       </c>
-      <c r="Q5" s="47">
+      <c r="Q5" s="28">
         <v>2014</v>
       </c>
-      <c r="R5" s="47">
+      <c r="R5" s="28">
         <v>2015</v>
       </c>
-      <c r="S5" s="47">
+      <c r="S5" s="28">
         <v>2016</v>
       </c>
-      <c r="T5" s="47">
+      <c r="T5" s="28">
         <v>2017</v>
       </c>
-      <c r="U5" s="47">
+      <c r="U5" s="28">
         <v>2018</v>
       </c>
-      <c r="V5" s="47">
+      <c r="V5" s="28">
         <v>2019</v>
       </c>
-      <c r="W5" s="47">
+      <c r="W5" s="28">
         <v>2020</v>
       </c>
-      <c r="X5" s="47">
+      <c r="X5" s="28">
         <v>2021</v>
       </c>
-      <c r="Y5" s="47">
+      <c r="Y5" s="28">
         <v>2022</v>
       </c>
-      <c r="Z5" s="47">
+      <c r="Z5" s="28">
         <v>2023</v>
       </c>
-      <c r="AA5" s="26"/>
-      <c r="AB5" s="26"/>
-      <c r="AC5" s="26"/>
-      <c r="AD5" s="26"/>
-      <c r="AE5" s="26"/>
-      <c r="AF5" s="26"/>
-      <c r="AG5" s="26"/>
-      <c r="AH5" s="26"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="26"/>
-      <c r="AK5" s="26"/>
-      <c r="AL5" s="26"/>
-      <c r="AM5" s="26"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="18"/>
+      <c r="AM5" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4189,720 +2982,720 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="23.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="18">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="10">
         <v>2018</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="10">
         <v>2023</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="E2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>46</v>
+      <c r="I2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="16">
+      <c r="A3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="51" t="e">
+      <c r="C3" s="29" t="e">
+        <f>IF(HPOPdata!F9&lt;&gt;"",HPOPdata!F9,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D3" s="29" t="e">
         <f>IF(HPOPdata!G9&lt;&gt;"",HPOPdata!G9,#N/A)</f>
         <v>#N/A</v>
       </c>
-      <c r="D3" s="51" t="e">
-        <f>IF(HPOPdata!H9&lt;&gt;"",HPOPdata!H9,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E3" s="51" t="e">
+      <c r="E3" s="29" t="e">
         <f>IF(OR(D3-C3&gt;0),D3,#N/A)</f>
         <v>#N/A</v>
       </c>
-      <c r="F3" s="51" t="e">
+      <c r="F3" s="29" t="e">
         <f>IF(D3-C3&lt;0,D3,#N/A)</f>
         <v>#N/A</v>
       </c>
-      <c r="G3" s="51" t="e">
+      <c r="G3" s="29" t="e">
         <f>IF(D3-C3&gt;0,D3-C3,#N/A)</f>
         <v>#N/A</v>
       </c>
-      <c r="H3" s="51" t="e">
+      <c r="H3" s="29" t="e">
         <f>IF(D3-C3&lt;0,ABS(D3-C3),#N/A)</f>
         <v>#N/A</v>
       </c>
-      <c r="I3" s="52" t="e">
-        <f>IF(HPOPdata!T9&lt;&gt;"",HPOPdata!T9,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J3" s="53">
-        <f>HPOPdata!U9</f>
+      <c r="I3" s="30" t="e">
+        <f>IF(HPOPdata!S9&lt;&gt;"",HPOPdata!S9,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J3" s="31">
+        <f>HPOPdata!T9</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="29" t="e">
+        <f>IF(HPOPdata!F10&lt;&gt;"",HPOPdata!F10,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D4" s="29" t="e">
+        <f>IF(HPOPdata!G10&lt;&gt;"",HPOPdata!G10,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E4" s="29" t="e">
+        <f t="shared" ref="E4:E19" si="0">IF(OR(D4-C4&gt;0),D4,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F4" s="29" t="e">
+        <f t="shared" ref="F4:F19" si="1">IF(D4-C4&lt;0,D4,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G4" s="29" t="e">
+        <f t="shared" ref="G4:G19" si="2">IF(D4-C4&gt;0,D4-C4,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H4" s="29" t="e">
+        <f t="shared" ref="H4:H19" si="3">IF(D4-C4&lt;0,ABS(D4-C4),#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I4" s="30" t="e">
+        <f>IF(HPOPdata!S10&lt;&gt;"",HPOPdata!S10,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J4" s="31">
+        <f>HPOPdata!T10</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="33"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="29" t="e">
+        <f>IF(HPOPdata!F11&lt;&gt;"",HPOPdata!F11,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D5" s="29" t="e">
+        <f>IF(HPOPdata!G11&lt;&gt;"",HPOPdata!G11,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E5" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F5" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G5" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H5" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="30" t="e">
+        <f>IF(HPOPdata!S11&lt;&gt;"",HPOPdata!S11,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J5" s="31">
+        <f>HPOPdata!T11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="29" t="e">
+        <f>IF(HPOPdata!F12&lt;&gt;"",HPOPdata!F12,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D6" s="29" t="e">
+        <f>IF(HPOPdata!G12&lt;&gt;"",HPOPdata!G12,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E6" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G6" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I6" s="30" t="e">
+        <f>IF(HPOPdata!S12&lt;&gt;"",HPOPdata!S12,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="31">
+        <f>HPOPdata!T12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="29" t="e">
+        <f>IF(HPOPdata!F13&lt;&gt;"",HPOPdata!F13,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D7" s="29" t="e">
+        <f>IF(HPOPdata!G13&lt;&gt;"",HPOPdata!G13,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E7" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F7" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G7" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H7" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I7" s="30" t="e">
+        <f>IF(HPOPdata!S13&lt;&gt;"",HPOPdata!S13,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J7" s="31">
+        <f>HPOPdata!T13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="29" t="e">
+        <f>IF(HPOPdata!F14&lt;&gt;"",HPOPdata!F14,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D8" s="29" t="e">
+        <f>IF(HPOPdata!G14&lt;&gt;"",HPOPdata!G14,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E8" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F8" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G8" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H8" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I8" s="30" t="e">
+        <f>IF(HPOPdata!S14&lt;&gt;"",HPOPdata!S14,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J8" s="31">
+        <f>HPOPdata!T14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="C9" s="29" t="e">
+        <f>IF(HPOPdata!F15&lt;&gt;"",HPOPdata!F15,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D9" s="29" t="e">
+        <f>IF(HPOPdata!G15&lt;&gt;"",HPOPdata!G15,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E9" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F9" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G9" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H9" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I9" s="30" t="e">
+        <f>IF(HPOPdata!S15&lt;&gt;"",HPOPdata!S15,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J9" s="31">
+        <f>HPOPdata!T15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="C10" s="29" t="e">
+        <f>IF(HPOPdata!F16&lt;&gt;"",HPOPdata!F16,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D10" s="29" t="e">
+        <f>IF(HPOPdata!G16&lt;&gt;"",HPOPdata!G16,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E10" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F10" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G10" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H10" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I10" s="30" t="e">
+        <f>IF(HPOPdata!S16&lt;&gt;"",HPOPdata!S16,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J10" s="31">
+        <f>HPOPdata!T16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="16">
-        <v>2</v>
-      </c>
-      <c r="C4" s="51" t="e">
-        <f>IF(HPOPdata!G10&lt;&gt;"",HPOPdata!G10,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D4" s="51" t="e">
-        <f>IF(HPOPdata!H10&lt;&gt;"",HPOPdata!H10,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E4" s="51" t="e">
-        <f t="shared" ref="E4:E19" si="0">IF(OR(D4-C4&gt;0),D4,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F4" s="51" t="e">
-        <f t="shared" ref="F4:F19" si="1">IF(D4-C4&lt;0,D4,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G4" s="51" t="e">
-        <f t="shared" ref="G4:G19" si="2">IF(D4-C4&gt;0,D4-C4,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H4" s="51" t="e">
-        <f t="shared" ref="H4:H19" si="3">IF(D4-C4&lt;0,ABS(D4-C4),#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I4" s="52" t="e">
-        <f>IF(HPOPdata!T10&lt;&gt;"",HPOPdata!T10,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J4" s="53">
-        <f>HPOPdata!U10</f>
+      <c r="B11" s="8">
+        <v>9</v>
+      </c>
+      <c r="C11" s="29" t="e">
+        <f>IF(HPOPdata!F17&lt;&gt;"",HPOPdata!F17,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D11" s="29" t="e">
+        <f>IF(HPOPdata!G17&lt;&gt;"",HPOPdata!G17,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E11" s="29" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" s="29" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G11" s="29" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="H11" s="29" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="I11" s="30" t="e">
+        <f>IF(HPOPdata!S17&lt;&gt;"",HPOPdata!S17,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J11" s="31">
+        <f>HPOPdata!T17</f>
         <v>0</v>
       </c>
-      <c r="L4" s="55"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="19" t="s">
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="16">
-        <v>3</v>
-      </c>
-      <c r="C5" s="51" t="e">
-        <f>IF(HPOPdata!G11&lt;&gt;"",HPOPdata!G11,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D5" s="51" t="e">
-        <f>IF(HPOPdata!H11&lt;&gt;"",HPOPdata!H11,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E5" s="51" t="e">
+      <c r="B12" s="8">
+        <v>10</v>
+      </c>
+      <c r="C12" s="29" t="e">
+        <f>IF(HPOPdata!F18&lt;&gt;"",HPOPdata!F18,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D12" s="29" t="e">
+        <f>IF(HPOPdata!G18&lt;&gt;"",HPOPdata!G18,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E12" s="29" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F5" s="51" t="e">
+      <c r="F12" s="29" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G5" s="51" t="e">
+      <c r="G12" s="29" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="H5" s="51" t="e">
+      <c r="H12" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I5" s="52" t="e">
-        <f>IF(HPOPdata!T11&lt;&gt;"",HPOPdata!T11,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J5" s="53">
-        <f>HPOPdata!U11</f>
+      <c r="I12" s="30" t="e">
+        <f>IF(HPOPdata!S18&lt;&gt;"",HPOPdata!S18,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J12" s="31">
+        <f>HPOPdata!T18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="19" t="s">
+    <row r="13" spans="1:12">
+      <c r="A13" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="16">
-        <v>4</v>
-      </c>
-      <c r="C6" s="51" t="e">
-        <f>IF(HPOPdata!G12&lt;&gt;"",HPOPdata!G12,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D6" s="51" t="e">
-        <f>IF(HPOPdata!H12&lt;&gt;"",HPOPdata!H12,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E6" s="51" t="e">
+      <c r="B13" s="8">
+        <v>11</v>
+      </c>
+      <c r="C13" s="29" t="e">
+        <f>IF(HPOPdata!F19&lt;&gt;"",HPOPdata!F19,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D13" s="29" t="e">
+        <f>IF(HPOPdata!G19&lt;&gt;"",HPOPdata!G19,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E13" s="29" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F6" s="51" t="e">
+      <c r="F13" s="29" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G6" s="51" t="e">
+      <c r="G13" s="29" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="H6" s="51" t="e">
+      <c r="H13" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I6" s="52" t="e">
-        <f>IF(HPOPdata!T12&lt;&gt;"",HPOPdata!T12,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J6" s="53">
-        <f>HPOPdata!U12</f>
+      <c r="I13" s="30" t="e">
+        <f>IF(HPOPdata!S19&lt;&gt;"",HPOPdata!S19,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J13" s="31">
+        <f>HPOPdata!T19</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="19" t="s">
+    <row r="14" spans="1:12">
+      <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="16">
-        <v>5</v>
-      </c>
-      <c r="C7" s="51" t="e">
-        <f>IF(HPOPdata!G13&lt;&gt;"",HPOPdata!G13,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D7" s="51" t="e">
-        <f>IF(HPOPdata!H13&lt;&gt;"",HPOPdata!H13,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E7" s="51" t="e">
+      <c r="B14" s="8">
+        <v>12</v>
+      </c>
+      <c r="C14" s="29" t="e">
+        <f>IF(HPOPdata!F20&lt;&gt;"",HPOPdata!F20,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D14" s="29" t="e">
+        <f>IF(HPOPdata!G20&lt;&gt;"",HPOPdata!G20,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E14" s="29" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F7" s="51" t="e">
+      <c r="F14" s="29" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G7" s="51" t="e">
+      <c r="G14" s="29" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="H7" s="51" t="e">
+      <c r="H14" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I7" s="52" t="e">
-        <f>IF(HPOPdata!T13&lt;&gt;"",HPOPdata!T13,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J7" s="53">
-        <f>HPOPdata!U13</f>
+      <c r="I14" s="30" t="e">
+        <f>IF(HPOPdata!S20&lt;&gt;"",HPOPdata!S20,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J14" s="31">
+        <f>HPOPdata!T20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="19" t="s">
+    <row r="15" spans="1:12">
+      <c r="A15" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="16">
-        <v>6</v>
-      </c>
-      <c r="C8" s="51" t="e">
-        <f>IF(HPOPdata!G14&lt;&gt;"",HPOPdata!G14,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D8" s="51" t="e">
-        <f>IF(HPOPdata!H14&lt;&gt;"",HPOPdata!H14,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E8" s="51" t="e">
+      <c r="B15" s="8">
+        <v>13</v>
+      </c>
+      <c r="C15" s="29" t="e">
+        <f>IF(HPOPdata!F21&lt;&gt;"",HPOPdata!F21,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D15" s="29" t="e">
+        <f>IF(HPOPdata!G21&lt;&gt;"",HPOPdata!G21,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E15" s="29" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F8" s="51" t="e">
+      <c r="F15" s="29" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G8" s="51" t="e">
+      <c r="G15" s="29" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="H8" s="51" t="e">
+      <c r="H15" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I8" s="52" t="e">
-        <f>IF(HPOPdata!T14&lt;&gt;"",HPOPdata!T14,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J8" s="53">
-        <f>HPOPdata!U14</f>
+      <c r="I15" s="30" t="e">
+        <f>IF(HPOPdata!S21&lt;&gt;"",HPOPdata!S21,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J15" s="31">
+        <f>HPOPdata!T21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="19" t="s">
+    <row r="16" spans="1:12">
+      <c r="A16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="16">
-        <v>7</v>
-      </c>
-      <c r="C9" s="51" t="e">
-        <f>IF(HPOPdata!G15&lt;&gt;"",HPOPdata!G15,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D9" s="51" t="e">
-        <f>IF(HPOPdata!H15&lt;&gt;"",HPOPdata!H15,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E9" s="51" t="e">
+      <c r="B16" s="8">
+        <v>14</v>
+      </c>
+      <c r="C16" s="29" t="e">
+        <f>IF(HPOPdata!F22&lt;&gt;"",HPOPdata!F22,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D16" s="29" t="e">
+        <f>IF(HPOPdata!G22&lt;&gt;"",HPOPdata!G22,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E16" s="29" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F9" s="51" t="e">
+      <c r="F16" s="29" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G9" s="51" t="e">
+      <c r="G16" s="29" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="H9" s="51" t="e">
+      <c r="H16" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I9" s="52" t="e">
-        <f>IF(HPOPdata!T15&lt;&gt;"",HPOPdata!T15,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J9" s="53">
-        <f>HPOPdata!U15</f>
+      <c r="I16" s="30" t="e">
+        <f>IF(HPOPdata!S22&lt;&gt;"",HPOPdata!S22,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J16" s="31">
+        <f>HPOPdata!T22</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="19" t="s">
+    <row r="17" spans="1:10">
+      <c r="A17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="16">
-        <v>8</v>
-      </c>
-      <c r="C10" s="51" t="e">
-        <f>IF(HPOPdata!G16&lt;&gt;"",HPOPdata!G16,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D10" s="51" t="e">
-        <f>IF(HPOPdata!H16&lt;&gt;"",HPOPdata!H16,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E10" s="51" t="e">
+      <c r="B17" s="8">
+        <v>15</v>
+      </c>
+      <c r="C17" s="29" t="e">
+        <f>IF(HPOPdata!F23&lt;&gt;"",HPOPdata!F23,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D17" s="29" t="e">
+        <f>IF(HPOPdata!G23&lt;&gt;"",HPOPdata!G23,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E17" s="29" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F10" s="51" t="e">
+      <c r="F17" s="29" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G10" s="51" t="e">
+      <c r="G17" s="29" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="H10" s="51" t="e">
+      <c r="H17" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I10" s="52" t="e">
-        <f>IF(HPOPdata!T16&lt;&gt;"",HPOPdata!T16,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J10" s="53">
-        <f>HPOPdata!U16</f>
+      <c r="I17" s="30" t="e">
+        <f>IF(HPOPdata!S23&lt;&gt;"",HPOPdata!S23,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J17" s="31">
+        <f>HPOPdata!T23</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="19" t="s">
+    <row r="18" spans="1:10">
+      <c r="A18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="16">
-        <v>9</v>
-      </c>
-      <c r="C11" s="51" t="e">
-        <f>IF(HPOPdata!G17&lt;&gt;"",HPOPdata!G17,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D11" s="51" t="e">
-        <f>IF(HPOPdata!H17&lt;&gt;"",HPOPdata!H17,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E11" s="51" t="e">
+      <c r="B18" s="8">
+        <v>16</v>
+      </c>
+      <c r="C18" s="29" t="e">
+        <f>IF(HPOPdata!F24&lt;&gt;"",HPOPdata!F24,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D18" s="29" t="e">
+        <f>IF(HPOPdata!G24&lt;&gt;"",HPOPdata!G24,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E18" s="29" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
-      <c r="F11" s="51" t="e">
+      <c r="F18" s="29" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="G11" s="51" t="e">
+      <c r="G18" s="29" t="e">
         <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="H11" s="51" t="e">
+      <c r="H18" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
-      <c r="I11" s="52" t="e">
-        <f>IF(HPOPdata!T17&lt;&gt;"",HPOPdata!T17,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J11" s="53">
-        <f>HPOPdata!U17</f>
+      <c r="I18" s="30" t="e">
+        <f>IF(HPOPdata!S24&lt;&gt;"",HPOPdata!S24,#N/A)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J18" s="31">
+        <f>HPOPdata!T24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="19" t="s">
+    <row r="19" spans="1:10">
+      <c r="A19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="16">
-        <v>10</v>
-      </c>
-      <c r="C12" s="51" t="e">
-        <f>IF(HPOPdata!G18&lt;&gt;"",HPOPdata!G18,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D12" s="51" t="e">
-        <f>IF(HPOPdata!H18&lt;&gt;"",HPOPdata!H18,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E12" s="51" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F12" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G12" s="51" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H12" s="51" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I12" s="52" t="e">
-        <f>IF(HPOPdata!T18&lt;&gt;"",HPOPdata!T18,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J12" s="53">
-        <f>HPOPdata!U18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="16">
-        <v>11</v>
-      </c>
-      <c r="C13" s="51" t="e">
-        <f>IF(HPOPdata!G19&lt;&gt;"",HPOPdata!G19,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D13" s="51" t="e">
-        <f>IF(HPOPdata!H19&lt;&gt;"",HPOPdata!H19,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E13" s="51" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F13" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G13" s="51" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H13" s="51" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I13" s="52" t="e">
-        <f>IF(HPOPdata!T19&lt;&gt;"",HPOPdata!T19,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J13" s="53">
-        <f>HPOPdata!U19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="16">
-        <v>12</v>
-      </c>
-      <c r="C14" s="51" t="e">
-        <f>IF(HPOPdata!G20&lt;&gt;"",HPOPdata!G20,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D14" s="51" t="e">
-        <f>IF(HPOPdata!H20&lt;&gt;"",HPOPdata!H20,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E14" s="51" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F14" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G14" s="51" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H14" s="51" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I14" s="52" t="e">
-        <f>IF(HPOPdata!T20&lt;&gt;"",HPOPdata!T20,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J14" s="53">
-        <f>HPOPdata!U20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="16">
-        <v>13</v>
-      </c>
-      <c r="C15" s="51" t="e">
-        <f>IF(HPOPdata!G21&lt;&gt;"",HPOPdata!G21,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D15" s="51" t="e">
-        <f>IF(HPOPdata!H21&lt;&gt;"",HPOPdata!H21,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E15" s="51" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F15" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G15" s="51" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H15" s="51" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I15" s="52" t="e">
-        <f>IF(HPOPdata!T21&lt;&gt;"",HPOPdata!T21,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J15" s="53">
-        <f>HPOPdata!U21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="16">
-        <v>14</v>
-      </c>
-      <c r="C16" s="51" t="e">
-        <f>IF(HPOPdata!G22&lt;&gt;"",HPOPdata!G22,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D16" s="51" t="e">
-        <f>IF(HPOPdata!H22&lt;&gt;"",HPOPdata!H22,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E16" s="51" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F16" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G16" s="51" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H16" s="51" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I16" s="52" t="e">
-        <f>IF(HPOPdata!T22&lt;&gt;"",HPOPdata!T22,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J16" s="53">
-        <f>HPOPdata!U22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="16">
-        <v>15</v>
-      </c>
-      <c r="C17" s="51" t="e">
-        <f>IF(HPOPdata!G23&lt;&gt;"",HPOPdata!G23,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D17" s="51" t="e">
-        <f>IF(HPOPdata!H23&lt;&gt;"",HPOPdata!H23,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E17" s="51" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F17" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G17" s="51" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H17" s="51" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I17" s="52" t="e">
-        <f>IF(HPOPdata!T23&lt;&gt;"",HPOPdata!T23,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J17" s="53">
-        <f>HPOPdata!U23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="16">
-        <v>16</v>
-      </c>
-      <c r="C18" s="51" t="e">
-        <f>IF(HPOPdata!G24&lt;&gt;"",HPOPdata!G24,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D18" s="51" t="e">
-        <f>IF(HPOPdata!H24&lt;&gt;"",HPOPdata!H24,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E18" s="51" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="F18" s="51" t="e">
-        <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="G18" s="51" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
-      </c>
-      <c r="H18" s="51" t="e">
-        <f t="shared" si="3"/>
-        <v>#N/A</v>
-      </c>
-      <c r="I18" s="52" t="e">
-        <f>IF(HPOPdata!T24&lt;&gt;"",HPOPdata!T24,#N/A)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J18" s="53">
-        <f>HPOPdata!U24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="16">
+      <c r="B19" s="8">
         <v>17</v>
       </c>
-      <c r="C19" s="51" t="e">
+      <c r="C19" s="29" t="e">
         <f>IF(HPOPdata!#REF!&lt;&gt;"",HPOPdata!#REF!,#N/A)</f>
         <v>#REF!</v>
       </c>
-      <c r="D19" s="51" t="e">
+      <c r="D19" s="29" t="e">
         <f>IF(HPOPdata!#REF!&lt;&gt;"",HPOPdata!#REF!,#N/A)</f>
         <v>#REF!</v>
       </c>
-      <c r="E19" s="51" t="e">
+      <c r="E19" s="29" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="F19" s="51" t="e">
+      <c r="F19" s="29" t="e">
         <f t="shared" si="1"/>
         <v>#REF!</v>
       </c>
-      <c r="G19" s="51" t="e">
+      <c r="G19" s="29" t="e">
         <f t="shared" si="2"/>
         <v>#REF!</v>
       </c>
-      <c r="H19" s="51" t="e">
+      <c r="H19" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#REF!</v>
       </c>
-      <c r="I19" s="52" t="e">
+      <c r="I19" s="30" t="e">
         <f>IF(HPOPdata!#REF!&lt;&gt;"",HPOPdata!#REF!,#N/A)</f>
         <v>#REF!</v>
       </c>
-      <c r="J19" s="53" t="e">
+      <c r="J19" s="31" t="e">
         <f>HPOPdata!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="B20" s="9"/>
+      <c r="B20" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4922,7 +3715,7 @@
   <cols>
     <col min="1" max="1" width="0.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="92.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
@@ -4931,365 +3724,365 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="30" customHeight="1">
-      <c r="B2" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="B3" s="20"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="17"/>
-      <c r="B4" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="54" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>67</v>
+      <c r="A4" s="9"/>
+      <c r="B4" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="17"/>
+      <c r="A5" s="9"/>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="B6" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="B8" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="B10" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="F13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="B14" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="B16" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="F20" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -5299,8 +4092,8 @@
       <c r="C22"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="42" t="s">
-        <v>54</v>
+      <c r="B23" s="23" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -5316,6 +4109,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -5532,15 +4334,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
   <ds:schemaRefs>
@@ -5558,6 +4351,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B07A0A-C848-4FF7-A830-0D9B654DA189}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5574,12 +4375,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixing HPOP export to excel functions to work with new summarising functions
</commit_message>
<xml_diff>
--- a/data-raw/CountrySummary_Template.xlsx
+++ b/data-raw/CountrySummary_Template.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D19D398-582C-40B0-BDF1-E4C62339FA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7399C187-00D2-41E1-AE45-755EE1FDF2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="17640" tabRatio="601" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="17640" tabRatio="601" activeTab="4" xr2:uid="{A0469F42-B2BF-41E9-9270-FEA8E2D23640}"/>
   </bookViews>
   <sheets>
-    <sheet name="HPOPdata" sheetId="11" r:id="rId1"/>
-    <sheet name="HPOPChart" sheetId="6" r:id="rId2"/>
-    <sheet name="HPOPTime Series" sheetId="8" r:id="rId3"/>
-    <sheet name="HPOPInter" sheetId="5" r:id="rId4"/>
-    <sheet name="HPOPIndicator List" sheetId="7" r:id="rId5"/>
+    <sheet name="data" sheetId="11" r:id="rId1"/>
+    <sheet name="Chart" sheetId="6" r:id="rId2"/>
+    <sheet name="Time Series" sheetId="8" r:id="rId3"/>
+    <sheet name="Inter" sheetId="5" r:id="rId4"/>
+    <sheet name="Indicator List" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HPOPdata!$A$1:$Q$25</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">data!$A$1:$Q$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -705,7 +705,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>HPOPInter!$E$2</c:f>
+              <c:f>Inter!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -761,7 +761,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>HPOPInter!$G$3:$G$19</c:f>
+                <c:f>Inter!$G$3:$G$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
@@ -829,7 +829,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>HPOPInter!$B$3:$B$19</c:f>
+              <c:f>Inter!$B$3:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -889,7 +889,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>HPOPInter!$E$3:$E$19</c:f>
+              <c:f>Inter!$E$3:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -959,7 +959,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>HPOPInter!$F$2</c:f>
+              <c:f>Inter!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -997,7 +997,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>HPOPInter!$H$3:$H$19</c:f>
+                <c:f>Inter!$H$3:$H$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
@@ -1057,7 +1057,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>HPOPInter!$H$3:$H$19</c:f>
+                <c:f>Inter!$H$3:$H$19</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="17"/>
@@ -1125,7 +1125,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>HPOPInter!$B$3:$B$19</c:f>
+              <c:f>Inter!$B$3:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1185,7 +1185,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>HPOPInter!$F$3:$F$19</c:f>
+              <c:f>Inter!$F$3:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1255,7 +1255,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>HPOPInter!$I$2</c:f>
+              <c:f>Inter!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1753,7 +1753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6071C4AC-2F6D-4B20-A20D-30CCF9C33A66}" type="CELLRANGE">
+                    <a:fld id="{F509903E-B556-4D14-89CC-FC17B1FAEEEC}" type="CELLRANGE">
                       <a:rPr lang="en-CH"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1837,7 +1837,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>HPOPInter!$B$3:$B$19</c:f>
+              <c:f>Inter!$B$3:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1897,7 +1897,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>HPOPInter!$I$3:$I$19</c:f>
+              <c:f>Inter!$I$3:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="17"/>
@@ -1959,7 +1959,7 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>HPOPInter!$J$3:$J$19</c15:f>
+                <c15:f>Inter!$J$3:$J$19</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="17"/>
                   <c:pt idx="0">
@@ -2526,8 +2526,8 @@
   </sheetPr>
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2648,71 +2648,71 @@
     <row r="22" spans="2:20" ht="162" customHeight="1">
       <c r="B22" s="7"/>
       <c r="C22" s="6" t="str">
-        <f>HPOPInter!A3</f>
+        <f>Inter!A3</f>
         <v>Children not stunted</v>
       </c>
       <c r="D22" s="6" t="str">
-        <f>HPOPInter!A4</f>
+        <f>Inter!A4</f>
         <v>Children not wasted</v>
       </c>
       <c r="E22" s="6" t="str">
-        <f>HPOPInter!A5</f>
+        <f>Inter!A5</f>
         <v>Children not overweight</v>
       </c>
       <c r="F22" s="6" t="str">
-        <f>HPOPInter!A6</f>
+        <f>Inter!A6</f>
         <v>Developmentally on track under 5</v>
       </c>
       <c r="G22" s="6" t="str">
-        <f>HPOPInter!A7</f>
+        <f>Inter!A7</f>
         <v>Children not obese</v>
       </c>
       <c r="H22" s="6" t="str">
-        <f>HPOPInter!A8</f>
+        <f>Inter!A8</f>
         <v>Reduced partner violence</v>
       </c>
       <c r="I22" s="6" t="str">
-        <f>HPOPInter!A9</f>
+        <f>Inter!A9</f>
         <v>Reduced child violence</v>
       </c>
       <c r="J22" s="6" t="str">
-        <f>HPOPInter!A10</f>
+        <f>Inter!A10</f>
         <v>Reduced suicide attempts</v>
       </c>
       <c r="K22" s="6" t="str">
-        <f>HPOPInter!A11</f>
+        <f>Inter!A11</f>
         <v>Road safety</v>
       </c>
       <c r="L22" s="6" t="str">
-        <f>HPOPInter!A12</f>
+        <f>Inter!A12</f>
         <v>Safely managed water</v>
       </c>
       <c r="M22" s="6" t="str">
-        <f>HPOPInter!A13</f>
+        <f>Inter!A13</f>
         <v>Safely managed sanitation</v>
       </c>
       <c r="N22" s="6" t="str">
-        <f>HPOPInter!A14</f>
+        <f>Inter!A14</f>
         <v>Clean household fuels</v>
       </c>
       <c r="O22" s="6" t="str">
-        <f>HPOPInter!A15</f>
+        <f>Inter!A15</f>
         <v>Reduced alcohol use</v>
       </c>
       <c r="P22" s="6" t="str">
-        <f>HPOPInter!A16</f>
+        <f>Inter!A16</f>
         <v>Ambient air quality</v>
       </c>
       <c r="Q22" s="6" t="str">
-        <f>HPOPInter!A17</f>
+        <f>Inter!A17</f>
         <v>Tobacco non-use</v>
       </c>
       <c r="R22" s="6" t="str">
-        <f>HPOPInter!A18</f>
+        <f>Inter!A18</f>
         <v>Adults not obese</v>
       </c>
       <c r="S22" s="6" t="str">
-        <f>HPOPInter!A19</f>
+        <f>Inter!A19</f>
         <v>Healthy fats</v>
       </c>
       <c r="T22" s="7"/>
@@ -3021,11 +3021,11 @@
         <v>1</v>
       </c>
       <c r="C3" s="29" t="e">
-        <f>IF(HPOPdata!F9&lt;&gt;"",HPOPdata!F9,#N/A)</f>
+        <f>IF(data!F9&lt;&gt;"",data!F9,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D3" s="29" t="e">
-        <f>IF(HPOPdata!G9&lt;&gt;"",HPOPdata!G9,#N/A)</f>
+        <f>IF(data!G9&lt;&gt;"",data!G9,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E3" s="29" t="e">
@@ -3045,11 +3045,11 @@
         <v>#N/A</v>
       </c>
       <c r="I3" s="30" t="e">
-        <f>IF(HPOPdata!S9&lt;&gt;"",HPOPdata!S9,#N/A)</f>
+        <f>IF(data!S9&lt;&gt;"",data!S9,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J3" s="31">
-        <f>HPOPdata!T9</f>
+        <f>data!T9</f>
         <v>0</v>
       </c>
     </row>
@@ -3061,11 +3061,11 @@
         <v>2</v>
       </c>
       <c r="C4" s="29" t="e">
-        <f>IF(HPOPdata!F10&lt;&gt;"",HPOPdata!F10,#N/A)</f>
+        <f>IF(data!F10&lt;&gt;"",data!F10,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D4" s="29" t="e">
-        <f>IF(HPOPdata!G10&lt;&gt;"",HPOPdata!G10,#N/A)</f>
+        <f>IF(data!G10&lt;&gt;"",data!G10,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E4" s="29" t="e">
@@ -3085,11 +3085,11 @@
         <v>#N/A</v>
       </c>
       <c r="I4" s="30" t="e">
-        <f>IF(HPOPdata!S10&lt;&gt;"",HPOPdata!S10,#N/A)</f>
+        <f>IF(data!S10&lt;&gt;"",data!S10,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J4" s="31">
-        <f>HPOPdata!T10</f>
+        <f>data!T10</f>
         <v>0</v>
       </c>
       <c r="L4" s="33"/>
@@ -3102,11 +3102,11 @@
         <v>3</v>
       </c>
       <c r="C5" s="29" t="e">
-        <f>IF(HPOPdata!F11&lt;&gt;"",HPOPdata!F11,#N/A)</f>
+        <f>IF(data!F11&lt;&gt;"",data!F11,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D5" s="29" t="e">
-        <f>IF(HPOPdata!G11&lt;&gt;"",HPOPdata!G11,#N/A)</f>
+        <f>IF(data!G11&lt;&gt;"",data!G11,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E5" s="29" t="e">
@@ -3126,11 +3126,11 @@
         <v>#N/A</v>
       </c>
       <c r="I5" s="30" t="e">
-        <f>IF(HPOPdata!S11&lt;&gt;"",HPOPdata!S11,#N/A)</f>
+        <f>IF(data!S11&lt;&gt;"",data!S11,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J5" s="31">
-        <f>HPOPdata!T11</f>
+        <f>data!T11</f>
         <v>0</v>
       </c>
     </row>
@@ -3142,11 +3142,11 @@
         <v>4</v>
       </c>
       <c r="C6" s="29" t="e">
-        <f>IF(HPOPdata!F12&lt;&gt;"",HPOPdata!F12,#N/A)</f>
+        <f>IF(data!F12&lt;&gt;"",data!F12,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D6" s="29" t="e">
-        <f>IF(HPOPdata!G12&lt;&gt;"",HPOPdata!G12,#N/A)</f>
+        <f>IF(data!G12&lt;&gt;"",data!G12,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E6" s="29" t="e">
@@ -3166,11 +3166,11 @@
         <v>#N/A</v>
       </c>
       <c r="I6" s="30" t="e">
-        <f>IF(HPOPdata!S12&lt;&gt;"",HPOPdata!S12,#N/A)</f>
+        <f>IF(data!S12&lt;&gt;"",data!S12,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J6" s="31">
-        <f>HPOPdata!T12</f>
+        <f>data!T12</f>
         <v>0</v>
       </c>
     </row>
@@ -3182,11 +3182,11 @@
         <v>5</v>
       </c>
       <c r="C7" s="29" t="e">
-        <f>IF(HPOPdata!F13&lt;&gt;"",HPOPdata!F13,#N/A)</f>
+        <f>IF(data!F13&lt;&gt;"",data!F13,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D7" s="29" t="e">
-        <f>IF(HPOPdata!G13&lt;&gt;"",HPOPdata!G13,#N/A)</f>
+        <f>IF(data!G13&lt;&gt;"",data!G13,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E7" s="29" t="e">
@@ -3206,11 +3206,11 @@
         <v>#N/A</v>
       </c>
       <c r="I7" s="30" t="e">
-        <f>IF(HPOPdata!S13&lt;&gt;"",HPOPdata!S13,#N/A)</f>
+        <f>IF(data!S13&lt;&gt;"",data!S13,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J7" s="31">
-        <f>HPOPdata!T13</f>
+        <f>data!T13</f>
         <v>0</v>
       </c>
     </row>
@@ -3222,11 +3222,11 @@
         <v>6</v>
       </c>
       <c r="C8" s="29" t="e">
-        <f>IF(HPOPdata!F14&lt;&gt;"",HPOPdata!F14,#N/A)</f>
+        <f>IF(data!F14&lt;&gt;"",data!F14,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D8" s="29" t="e">
-        <f>IF(HPOPdata!G14&lt;&gt;"",HPOPdata!G14,#N/A)</f>
+        <f>IF(data!G14&lt;&gt;"",data!G14,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E8" s="29" t="e">
@@ -3246,11 +3246,11 @@
         <v>#N/A</v>
       </c>
       <c r="I8" s="30" t="e">
-        <f>IF(HPOPdata!S14&lt;&gt;"",HPOPdata!S14,#N/A)</f>
+        <f>IF(data!S14&lt;&gt;"",data!S14,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J8" s="31">
-        <f>HPOPdata!T14</f>
+        <f>data!T14</f>
         <v>0</v>
       </c>
     </row>
@@ -3262,11 +3262,11 @@
         <v>7</v>
       </c>
       <c r="C9" s="29" t="e">
-        <f>IF(HPOPdata!F15&lt;&gt;"",HPOPdata!F15,#N/A)</f>
+        <f>IF(data!F15&lt;&gt;"",data!F15,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D9" s="29" t="e">
-        <f>IF(HPOPdata!G15&lt;&gt;"",HPOPdata!G15,#N/A)</f>
+        <f>IF(data!G15&lt;&gt;"",data!G15,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E9" s="29" t="e">
@@ -3286,11 +3286,11 @@
         <v>#N/A</v>
       </c>
       <c r="I9" s="30" t="e">
-        <f>IF(HPOPdata!S15&lt;&gt;"",HPOPdata!S15,#N/A)</f>
+        <f>IF(data!S15&lt;&gt;"",data!S15,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J9" s="31">
-        <f>HPOPdata!T15</f>
+        <f>data!T15</f>
         <v>0</v>
       </c>
     </row>
@@ -3302,11 +3302,11 @@
         <v>8</v>
       </c>
       <c r="C10" s="29" t="e">
-        <f>IF(HPOPdata!F16&lt;&gt;"",HPOPdata!F16,#N/A)</f>
+        <f>IF(data!F16&lt;&gt;"",data!F16,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D10" s="29" t="e">
-        <f>IF(HPOPdata!G16&lt;&gt;"",HPOPdata!G16,#N/A)</f>
+        <f>IF(data!G16&lt;&gt;"",data!G16,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E10" s="29" t="e">
@@ -3326,11 +3326,11 @@
         <v>#N/A</v>
       </c>
       <c r="I10" s="30" t="e">
-        <f>IF(HPOPdata!S16&lt;&gt;"",HPOPdata!S16,#N/A)</f>
+        <f>IF(data!S16&lt;&gt;"",data!S16,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J10" s="31">
-        <f>HPOPdata!T16</f>
+        <f>data!T16</f>
         <v>0</v>
       </c>
     </row>
@@ -3342,11 +3342,11 @@
         <v>9</v>
       </c>
       <c r="C11" s="29" t="e">
-        <f>IF(HPOPdata!F17&lt;&gt;"",HPOPdata!F17,#N/A)</f>
+        <f>IF(data!F17&lt;&gt;"",data!F17,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D11" s="29" t="e">
-        <f>IF(HPOPdata!G17&lt;&gt;"",HPOPdata!G17,#N/A)</f>
+        <f>IF(data!G17&lt;&gt;"",data!G17,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E11" s="29" t="e">
@@ -3366,11 +3366,11 @@
         <v>#N/A</v>
       </c>
       <c r="I11" s="30" t="e">
-        <f>IF(HPOPdata!S17&lt;&gt;"",HPOPdata!S17,#N/A)</f>
+        <f>IF(data!S17&lt;&gt;"",data!S17,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J11" s="31">
-        <f>HPOPdata!T17</f>
+        <f>data!T17</f>
         <v>0</v>
       </c>
     </row>
@@ -3382,11 +3382,11 @@
         <v>10</v>
       </c>
       <c r="C12" s="29" t="e">
-        <f>IF(HPOPdata!F18&lt;&gt;"",HPOPdata!F18,#N/A)</f>
+        <f>IF(data!F18&lt;&gt;"",data!F18,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D12" s="29" t="e">
-        <f>IF(HPOPdata!G18&lt;&gt;"",HPOPdata!G18,#N/A)</f>
+        <f>IF(data!G18&lt;&gt;"",data!G18,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E12" s="29" t="e">
@@ -3406,11 +3406,11 @@
         <v>#N/A</v>
       </c>
       <c r="I12" s="30" t="e">
-        <f>IF(HPOPdata!S18&lt;&gt;"",HPOPdata!S18,#N/A)</f>
+        <f>IF(data!S18&lt;&gt;"",data!S18,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J12" s="31">
-        <f>HPOPdata!T18</f>
+        <f>data!T18</f>
         <v>0</v>
       </c>
     </row>
@@ -3422,11 +3422,11 @@
         <v>11</v>
       </c>
       <c r="C13" s="29" t="e">
-        <f>IF(HPOPdata!F19&lt;&gt;"",HPOPdata!F19,#N/A)</f>
+        <f>IF(data!F19&lt;&gt;"",data!F19,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D13" s="29" t="e">
-        <f>IF(HPOPdata!G19&lt;&gt;"",HPOPdata!G19,#N/A)</f>
+        <f>IF(data!G19&lt;&gt;"",data!G19,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E13" s="29" t="e">
@@ -3446,11 +3446,11 @@
         <v>#N/A</v>
       </c>
       <c r="I13" s="30" t="e">
-        <f>IF(HPOPdata!S19&lt;&gt;"",HPOPdata!S19,#N/A)</f>
+        <f>IF(data!S19&lt;&gt;"",data!S19,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J13" s="31">
-        <f>HPOPdata!T19</f>
+        <f>data!T19</f>
         <v>0</v>
       </c>
     </row>
@@ -3462,11 +3462,11 @@
         <v>12</v>
       </c>
       <c r="C14" s="29" t="e">
-        <f>IF(HPOPdata!F20&lt;&gt;"",HPOPdata!F20,#N/A)</f>
+        <f>IF(data!F20&lt;&gt;"",data!F20,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D14" s="29" t="e">
-        <f>IF(HPOPdata!G20&lt;&gt;"",HPOPdata!G20,#N/A)</f>
+        <f>IF(data!G20&lt;&gt;"",data!G20,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E14" s="29" t="e">
@@ -3486,11 +3486,11 @@
         <v>#N/A</v>
       </c>
       <c r="I14" s="30" t="e">
-        <f>IF(HPOPdata!S20&lt;&gt;"",HPOPdata!S20,#N/A)</f>
+        <f>IF(data!S20&lt;&gt;"",data!S20,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J14" s="31">
-        <f>HPOPdata!T20</f>
+        <f>data!T20</f>
         <v>0</v>
       </c>
     </row>
@@ -3502,11 +3502,11 @@
         <v>13</v>
       </c>
       <c r="C15" s="29" t="e">
-        <f>IF(HPOPdata!F21&lt;&gt;"",HPOPdata!F21,#N/A)</f>
+        <f>IF(data!F21&lt;&gt;"",data!F21,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D15" s="29" t="e">
-        <f>IF(HPOPdata!G21&lt;&gt;"",HPOPdata!G21,#N/A)</f>
+        <f>IF(data!G21&lt;&gt;"",data!G21,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E15" s="29" t="e">
@@ -3526,11 +3526,11 @@
         <v>#N/A</v>
       </c>
       <c r="I15" s="30" t="e">
-        <f>IF(HPOPdata!S21&lt;&gt;"",HPOPdata!S21,#N/A)</f>
+        <f>IF(data!S21&lt;&gt;"",data!S21,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J15" s="31">
-        <f>HPOPdata!T21</f>
+        <f>data!T21</f>
         <v>0</v>
       </c>
     </row>
@@ -3542,11 +3542,11 @@
         <v>14</v>
       </c>
       <c r="C16" s="29" t="e">
-        <f>IF(HPOPdata!F22&lt;&gt;"",HPOPdata!F22,#N/A)</f>
+        <f>IF(data!F22&lt;&gt;"",data!F22,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D16" s="29" t="e">
-        <f>IF(HPOPdata!G22&lt;&gt;"",HPOPdata!G22,#N/A)</f>
+        <f>IF(data!G22&lt;&gt;"",data!G22,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E16" s="29" t="e">
@@ -3566,11 +3566,11 @@
         <v>#N/A</v>
       </c>
       <c r="I16" s="30" t="e">
-        <f>IF(HPOPdata!S22&lt;&gt;"",HPOPdata!S22,#N/A)</f>
+        <f>IF(data!S22&lt;&gt;"",data!S22,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J16" s="31">
-        <f>HPOPdata!T22</f>
+        <f>data!T22</f>
         <v>0</v>
       </c>
     </row>
@@ -3582,11 +3582,11 @@
         <v>15</v>
       </c>
       <c r="C17" s="29" t="e">
-        <f>IF(HPOPdata!F23&lt;&gt;"",HPOPdata!F23,#N/A)</f>
+        <f>IF(data!F23&lt;&gt;"",data!F23,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D17" s="29" t="e">
-        <f>IF(HPOPdata!G23&lt;&gt;"",HPOPdata!G23,#N/A)</f>
+        <f>IF(data!G23&lt;&gt;"",data!G23,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E17" s="29" t="e">
@@ -3606,11 +3606,11 @@
         <v>#N/A</v>
       </c>
       <c r="I17" s="30" t="e">
-        <f>IF(HPOPdata!S23&lt;&gt;"",HPOPdata!S23,#N/A)</f>
+        <f>IF(data!S23&lt;&gt;"",data!S23,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J17" s="31">
-        <f>HPOPdata!T23</f>
+        <f>data!T23</f>
         <v>0</v>
       </c>
     </row>
@@ -3622,11 +3622,11 @@
         <v>16</v>
       </c>
       <c r="C18" s="29" t="e">
-        <f>IF(HPOPdata!F24&lt;&gt;"",HPOPdata!F24,#N/A)</f>
+        <f>IF(data!F24&lt;&gt;"",data!F24,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="D18" s="29" t="e">
-        <f>IF(HPOPdata!G24&lt;&gt;"",HPOPdata!G24,#N/A)</f>
+        <f>IF(data!G24&lt;&gt;"",data!G24,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="E18" s="29" t="e">
@@ -3646,11 +3646,11 @@
         <v>#N/A</v>
       </c>
       <c r="I18" s="30" t="e">
-        <f>IF(HPOPdata!S24&lt;&gt;"",HPOPdata!S24,#N/A)</f>
+        <f>IF(data!S24&lt;&gt;"",data!S24,#N/A)</f>
         <v>#N/A</v>
       </c>
       <c r="J18" s="31">
-        <f>HPOPdata!T24</f>
+        <f>data!T24</f>
         <v>0</v>
       </c>
     </row>
@@ -3662,11 +3662,11 @@
         <v>17</v>
       </c>
       <c r="C19" s="29" t="e">
-        <f>IF(HPOPdata!#REF!&lt;&gt;"",HPOPdata!#REF!,#N/A)</f>
+        <f>IF(data!#REF!&lt;&gt;"",data!#REF!,#N/A)</f>
         <v>#REF!</v>
       </c>
       <c r="D19" s="29" t="e">
-        <f>IF(HPOPdata!#REF!&lt;&gt;"",HPOPdata!#REF!,#N/A)</f>
+        <f>IF(data!#REF!&lt;&gt;"",data!#REF!,#N/A)</f>
         <v>#REF!</v>
       </c>
       <c r="E19" s="29" t="e">
@@ -3686,11 +3686,11 @@
         <v>#REF!</v>
       </c>
       <c r="I19" s="30" t="e">
-        <f>IF(HPOPdata!#REF!&lt;&gt;"",HPOPdata!#REF!,#N/A)</f>
+        <f>IF(data!#REF!&lt;&gt;"",data!#REF!,#N/A)</f>
         <v>#REF!</v>
       </c>
       <c r="J19" s="31" t="e">
-        <f>HPOPdata!#REF!</f>
+        <f>data!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF07AF5-FD4F-4F8B-8ACA-4EDEF61AF714}">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -4103,21 +4103,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAB383CFE351E4980079CAB43D24491" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21903c200076b3ec55be68dd2bdf11fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c" xmlns:ns3="bd879b36-96f5-4c4e-979a-9eb1cd712529" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f489635911e13f24b7b9894dba5432d9" ns2:_="" ns3:_="">
     <xsd:import namespace="1022376e-cd63-4e3a-9ae1-c617fc1c4f2c"/>
@@ -4334,31 +4319,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3B07A0A-C848-4FF7-A830-0D9B654DA189}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4375,4 +4351,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8C5798F-31D9-455C-A266-3CF2A88C6872}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cee211f1-5bf1-4f4b-adf1-18b7c5b9a3a6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5668EAE9-BE2F-449B-83FE-5638B2ED2DF4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>